<commit_message>
working on jags model and nimble model
trying to figure out if the detection intercepts or time since rain are causing the weird enes occupancy levels
</commit_message>
<xml_diff>
--- a/2020/2020_code_jayjones/osslist_metadata_JW.xlsx
+++ b/2020/2020_code_jayjones/osslist_metadata_JW.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/80ef66c4777addb1/Documents/Academic/OSU/Git/oss-occu/2020/2020_code_jayjones/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="192" documentId="8_{928031BB-0278-4684-980E-41D3D69863A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B682110-AFDC-4E2B-A426-3C0D00E3267A}"/>
+  <xr:revisionPtr revIDLastSave="280" documentId="8_{928031BB-0278-4684-980E-41D3D69863A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{574D3094-C5FD-AD4F-A6F0-E3A4C60C6231}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-1200" windowWidth="22780" windowHeight="14540" xr2:uid="{356F900B-4592-472C-A3A5-3F2F56E84E67}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19440" xr2:uid="{356F900B-4592-472C-A3A5-3F2F56E84E67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="127">
   <si>
     <t>nstand</t>
   </si>
@@ -293,9 +293,6 @@
     <t>numbers 1-7 repeated 88 times</t>
   </si>
   <si>
-    <t>7 for year or for subplot?</t>
-  </si>
-  <si>
     <t>7 years for each stand</t>
   </si>
   <si>
@@ -326,12 +323,6 @@
     <t>1's across row 7</t>
   </si>
   <si>
-    <t>length 616, one for each year?</t>
-  </si>
-  <si>
-    <t>not sure I understand how this was executed</t>
-  </si>
-  <si>
     <t>length 3379, one per plot? Incl repeats</t>
   </si>
   <si>
@@ -350,12 +341,6 @@
     <t>questions</t>
   </si>
   <si>
-    <t>1=pretrt? Or surveyed pre-trt?</t>
-  </si>
-  <si>
-    <t>1=post-trt? surveyed post-trt?</t>
-  </si>
-  <si>
     <t>occupancy matrix, dim 3379x3</t>
   </si>
   <si>
@@ -381,13 +366,64 @@
   </si>
   <si>
     <t>enes</t>
+  </si>
+  <si>
+    <t>Factor w/ 3 levels (Control, PostTrt, PreTrt)</t>
+  </si>
+  <si>
+    <t>1 1 1 1 1 1 1 1 1 1 …</t>
+  </si>
+  <si>
+    <t>1=pre-trt survey year</t>
+  </si>
+  <si>
+    <t>1=post-trt survey year</t>
+  </si>
+  <si>
+    <t>years, stand level</t>
+  </si>
+  <si>
+    <t>length 616, one for each stand each year?</t>
+  </si>
+  <si>
+    <t>should only have to make the ones above- below are just repeats in a different format</t>
+  </si>
+  <si>
+    <t>how many stands now? Which are repeats? Do repeats matter?</t>
+  </si>
+  <si>
+    <t>same</t>
+  </si>
+  <si>
+    <t>just add mine (127*7*3=2667) to 3379?</t>
+  </si>
+  <si>
+    <t>easy, dep on num stands</t>
+  </si>
+  <si>
+    <t>change size num stands</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>" and add other tree farm option</t>
+  </si>
+  <si>
+    <t>to do</t>
+  </si>
+  <si>
+    <t>change size?</t>
+  </si>
+  <si>
+    <t>" and add matrices for my years</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -401,6 +437,13 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -466,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -492,18 +535,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -515,6 +549,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -531,10 +587,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -854,22 +906,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E728E407-9FE8-4495-B584-A5C64E1E4C89}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="42.7109375" customWidth="1"/>
-    <col min="5" max="5" width="41.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="28.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="35.6640625" customWidth="1"/>
+    <col min="5" max="5" width="39" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
+    <col min="7" max="7" width="61.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>65</v>
       </c>
@@ -883,13 +937,16 @@
         <v>68</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -900,13 +957,16 @@
         <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -920,8 +980,11 @@
         <v>70</v>
       </c>
       <c r="F3" s="9"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -935,8 +998,11 @@
         <v>71</v>
       </c>
       <c r="F4" s="9"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -950,8 +1016,11 @@
         <v>72</v>
       </c>
       <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -965,11 +1034,14 @@
         <v>75</v>
       </c>
       <c r="E6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -982,11 +1054,14 @@
       <c r="D7" t="s">
         <v>73</v>
       </c>
-      <c r="F7" s="17" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1002,9 +1077,12 @@
       <c r="E8" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="17"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="14"/>
+      <c r="G8" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1018,9 +1096,12 @@
         <v>77</v>
       </c>
       <c r="E9" s="10"/>
-      <c r="F9" s="17"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="14"/>
+      <c r="G9" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1034,9 +1115,12 @@
         <v>78</v>
       </c>
       <c r="E10" s="10"/>
-      <c r="F10" s="17"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="14"/>
+      <c r="G10" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -1052,163 +1136,184 @@
       <c r="E11" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F11" s="18"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="F11" s="15"/>
+      <c r="G11" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="7" t="s">
+      <c r="B18" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D18" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E18" s="16"/>
+      <c r="F18" s="20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" t="s">
-        <v>84</v>
-      </c>
-      <c r="E13" t="s">
-        <v>86</v>
-      </c>
-      <c r="F13" s="12"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" t="s">
-        <v>90</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="F14" s="12"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="12"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" t="s">
-        <v>92</v>
-      </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="12"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" t="s">
-        <v>93</v>
-      </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="12"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" t="s">
-        <v>94</v>
-      </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="12"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" t="s">
-        <v>95</v>
-      </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="12"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="20"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>110</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" t="s">
         <v>87</v>
       </c>
-      <c r="D20" t="s">
-        <v>88</v>
-      </c>
       <c r="E20" t="s">
-        <v>96</v>
-      </c>
-      <c r="F20" s="12"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="F20" s="20"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -1219,11 +1324,11 @@
         <v>34</v>
       </c>
       <c r="E21" t="s">
-        <v>104</v>
-      </c>
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="F21" s="20"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>35</v>
       </c>
@@ -1235,11 +1340,11 @@
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F22" s="13"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="F22" s="11"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>36</v>
       </c>
@@ -1253,13 +1358,16 @@
         <v>74</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1270,14 +1378,11 @@
         <v>69</v>
       </c>
       <c r="D24" t="s">
-        <v>89</v>
-      </c>
-      <c r="E24" t="s">
-        <v>97</v>
-      </c>
-      <c r="F24" s="15"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1288,11 +1393,11 @@
         <v>40</v>
       </c>
       <c r="E25" t="s">
-        <v>108</v>
-      </c>
-      <c r="F25" s="15"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="F25" s="12"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1302,9 +1407,9 @@
       <c r="C26" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F26" s="15"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -1314,9 +1419,9 @@
       <c r="C27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="15"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="12"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -1327,14 +1432,14 @@
         <v>46</v>
       </c>
       <c r="D28" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E28" t="s">
-        <v>113</v>
-      </c>
-      <c r="F28" s="15"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="F28" s="12"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -1345,11 +1450,11 @@
         <v>46</v>
       </c>
       <c r="D29" t="s">
-        <v>114</v>
-      </c>
-      <c r="F29" s="15"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="F29" s="12"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -1359,9 +1464,9 @@
       <c r="C30" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="15"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F30" s="12"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -1372,11 +1477,11 @@
         <v>50</v>
       </c>
       <c r="D31" t="s">
-        <v>107</v>
-      </c>
-      <c r="F31" s="15"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="F31" s="12"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>51</v>
       </c>
@@ -1386,9 +1491,9 @@
       <c r="C32" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F32" s="15"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="12"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -1398,9 +1503,9 @@
       <c r="C33" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F33" s="15"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="12"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -1410,9 +1515,9 @@
       <c r="C34" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F34" s="15"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="12"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -1423,11 +1528,11 @@
         <v>55</v>
       </c>
       <c r="E35" t="s">
-        <v>108</v>
-      </c>
-      <c r="F35" s="15"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="F35" s="12"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -1437,9 +1542,9 @@
       <c r="C36" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F36" s="15"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="12"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -1449,9 +1554,9 @@
       <c r="C37" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F37" s="15"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="12"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -1461,9 +1566,9 @@
       <c r="C38" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F38" s="15"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="12"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>59</v>
       </c>
@@ -1473,9 +1578,9 @@
       <c r="C39" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F39" s="15"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="12"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>60</v>
       </c>
@@ -1485,9 +1590,9 @@
       <c r="C40" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F40" s="15"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="12"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>61</v>
       </c>
@@ -1495,14 +1600,14 @@
         <v>64</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D41" t="s">
-        <v>101</v>
-      </c>
-      <c r="F41" s="15"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="F41" s="12"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>62</v>
       </c>
@@ -1512,9 +1617,9 @@
       <c r="C42" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F42" s="15"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F42" s="12"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>63</v>
       </c>
@@ -1526,16 +1631,16 @@
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
-      <c r="F43" s="16"/>
+      <c r="F43" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="F2:F6"/>
     <mergeCell ref="E8:E10"/>
-    <mergeCell ref="E14:E19"/>
-    <mergeCell ref="F12:F22"/>
+    <mergeCell ref="E12:E17"/>
     <mergeCell ref="F23:F43"/>
     <mergeCell ref="F7:F11"/>
+    <mergeCell ref="F18:F22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
separated nimble script into three scripts, cleaned
</commit_message>
<xml_diff>
--- a/2020/2020_code_jayjones/osslist_metadata_JW.xlsx
+++ b/2020/2020_code_jayjones/osslist_metadata_JW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/80ef66c4777addb1/Documents/Academic/OSU/Git/oss-occu/2020/2020_code_jayjones/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="280" documentId="8_{928031BB-0278-4684-980E-41D3D69863A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{574D3094-C5FD-AD4F-A6F0-E3A4C60C6231}"/>
+  <xr:revisionPtr revIDLastSave="291" documentId="8_{928031BB-0278-4684-980E-41D3D69863A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A263685-34C7-AD42-A00A-8BA839467E79}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19440" xr2:uid="{356F900B-4592-472C-A3A5-3F2F56E84E67}"/>
+    <workbookView xWindow="-38400" yWindow="1240" windowWidth="38400" windowHeight="21100" xr2:uid="{356F900B-4592-472C-A3A5-3F2F56E84E67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="130">
   <si>
     <t>nstand</t>
   </si>
@@ -329,9 +329,6 @@
     <t>variables with "2" include info for the stand and year level?</t>
   </si>
   <si>
-    <t>variables with "3" are a vector with info for each survey?</t>
-  </si>
-  <si>
     <t>length 3379</t>
   </si>
   <si>
@@ -362,9 +359,6 @@
     <t>7x88, year x stand. 2013=1, 2019=7. cell=1 if it was surveyed that year. But 88 plots werent sampled each year?</t>
   </si>
   <si>
-    <t>repeat surveys oss. Why NA's?</t>
-  </si>
-  <si>
     <t>enes</t>
   </si>
   <si>
@@ -417,6 +411,21 @@
   </si>
   <si>
     <t>" and add matrices for my years</t>
+  </si>
+  <si>
+    <t>treatment designation for each stand in each year</t>
+  </si>
+  <si>
+    <t>need to change to my treatments; add more matrices, 5treatments plus pre-harv?</t>
+  </si>
+  <si>
+    <t>variables with "3" are a vector with info for each survey replicate?</t>
+  </si>
+  <si>
+    <t>put my occupancy matrices in this format</t>
+  </si>
+  <si>
+    <t>repeat surveys oss. NA's, some werent surveyed 3x</t>
   </si>
 </sst>
 </file>
@@ -509,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -526,6 +535,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -534,9 +552,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -550,27 +565,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -587,6 +586,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -909,7 +912,7 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -937,13 +940,13 @@
         <v>68</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="23" t="s">
-        <v>124</v>
+      <c r="G1" s="10" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -957,13 +960,13 @@
         <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F2" s="8" t="s">
         <v>105</v>
       </c>
+      <c r="F2" s="11" t="s">
+        <v>104</v>
+      </c>
       <c r="G2" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -979,9 +982,9 @@
       <c r="D3" t="s">
         <v>70</v>
       </c>
-      <c r="F3" s="9"/>
+      <c r="F3" s="12"/>
       <c r="G3" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -997,7 +1000,7 @@
       <c r="D4" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="9"/>
+      <c r="F4" s="12"/>
       <c r="G4" s="1">
         <v>9</v>
       </c>
@@ -1015,9 +1018,9 @@
       <c r="D5" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="9"/>
+      <c r="F5" s="12"/>
       <c r="G5" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1034,11 +1037,11 @@
         <v>75</v>
       </c>
       <c r="E6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F6" s="9"/>
+        <v>98</v>
+      </c>
+      <c r="F6" s="12"/>
       <c r="G6" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1054,11 +1057,11 @@
       <c r="D7" t="s">
         <v>73</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>104</v>
+      <c r="F7" s="16" t="s">
+        <v>103</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1074,12 +1077,12 @@
       <c r="D8" t="s">
         <v>76</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="14"/>
+      <c r="F8" s="16"/>
       <c r="G8" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1095,10 +1098,10 @@
       <c r="D9" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="14"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="16"/>
       <c r="G9" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1114,10 +1117,10 @@
       <c r="D10" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="14"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="16"/>
       <c r="G10" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1136,9 +1139,9 @@
       <c r="E11" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F11" s="15"/>
+      <c r="F11" s="17"/>
       <c r="G11" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1154,12 +1157,12 @@
       <c r="D12" t="s">
         <v>89</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="F12" s="18"/>
+      <c r="E12" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="8"/>
       <c r="G12" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1175,10 +1178,10 @@
       <c r="D13" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="18"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1194,12 +1197,12 @@
       <c r="D14" t="s">
         <v>91</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="19" t="s">
-        <v>114</v>
+      <c r="E14" s="13"/>
+      <c r="F14" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1215,10 +1218,10 @@
       <c r="D15" t="s">
         <v>92</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="18"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1234,10 +1237,10 @@
       <c r="D16" t="s">
         <v>93</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="18"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="8"/>
       <c r="G16" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1253,65 +1256,73 @@
       <c r="D17" t="s">
         <v>94</v>
       </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="18"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="8"/>
       <c r="G17" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="16" t="s">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="17" t="s">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" t="s">
         <v>83</v>
       </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="18" t="s">
         <v>96</v>
       </c>
+      <c r="G18" s="1" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="16" t="s">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="17" t="s">
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" t="s">
         <v>84</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="20"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="1" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D20" t="s">
         <v>87</v>
       </c>
       <c r="E20" t="s">
-        <v>115</v>
-      </c>
-      <c r="F20" s="20"/>
+        <v>113</v>
+      </c>
+      <c r="F20" s="18"/>
+      <c r="G20" s="1" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -1324,9 +1335,12 @@
         <v>34</v>
       </c>
       <c r="E21" t="s">
-        <v>112</v>
-      </c>
-      <c r="F21" s="20"/>
+        <v>110</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
@@ -1340,9 +1354,12 @@
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="F22" s="11"/>
+        <v>111</v>
+      </c>
+      <c r="F22" s="19"/>
+      <c r="G22" s="5" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
@@ -1360,11 +1377,11 @@
       <c r="E23" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F23" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="G23" s="22" t="s">
-        <v>116</v>
+      <c r="F23" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1380,7 +1397,7 @@
       <c r="D24" t="s">
         <v>88</v>
       </c>
-      <c r="F24" s="12"/>
+      <c r="F24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -1393,9 +1410,9 @@
         <v>40</v>
       </c>
       <c r="E25" t="s">
-        <v>103</v>
-      </c>
-      <c r="F25" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F25" s="14"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -1407,7 +1424,7 @@
       <c r="C26" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F26" s="12"/>
+      <c r="F26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -1419,7 +1436,7 @@
       <c r="C27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="12"/>
+      <c r="F27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -1432,12 +1449,15 @@
         <v>46</v>
       </c>
       <c r="D28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E28" t="s">
-        <v>108</v>
-      </c>
-      <c r="F28" s="12"/>
+        <v>129</v>
+      </c>
+      <c r="F28" s="14"/>
+      <c r="G28" s="1" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -1450,9 +1470,12 @@
         <v>46</v>
       </c>
       <c r="D29" t="s">
-        <v>109</v>
-      </c>
-      <c r="F29" s="12"/>
+        <v>107</v>
+      </c>
+      <c r="F29" s="14"/>
+      <c r="G29" s="1" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -1464,7 +1487,7 @@
       <c r="C30" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="12"/>
+      <c r="F30" s="14"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -1477,9 +1500,9 @@
         <v>50</v>
       </c>
       <c r="D31" t="s">
-        <v>102</v>
-      </c>
-      <c r="F31" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="F31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -1491,7 +1514,7 @@
       <c r="C32" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F32" s="12"/>
+      <c r="F32" s="14"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
@@ -1503,7 +1526,7 @@
       <c r="C33" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F33" s="12"/>
+      <c r="F33" s="14"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
@@ -1515,7 +1538,7 @@
       <c r="C34" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F34" s="12"/>
+      <c r="F34" s="14"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
@@ -1528,9 +1551,9 @@
         <v>55</v>
       </c>
       <c r="E35" t="s">
-        <v>103</v>
-      </c>
-      <c r="F35" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F35" s="14"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
@@ -1542,7 +1565,7 @@
       <c r="C36" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F36" s="12"/>
+      <c r="F36" s="14"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
@@ -1554,7 +1577,7 @@
       <c r="C37" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F37" s="12"/>
+      <c r="F37" s="14"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
@@ -1566,7 +1589,7 @@
       <c r="C38" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F38" s="12"/>
+      <c r="F38" s="14"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
@@ -1578,7 +1601,7 @@
       <c r="C39" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F39" s="12"/>
+      <c r="F39" s="14"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
@@ -1590,7 +1613,7 @@
       <c r="C40" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F40" s="12"/>
+      <c r="F40" s="14"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
@@ -1603,9 +1626,9 @@
         <v>86</v>
       </c>
       <c r="D41" t="s">
-        <v>98</v>
-      </c>
-      <c r="F41" s="12"/>
+        <v>97</v>
+      </c>
+      <c r="F41" s="14"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
@@ -1617,7 +1640,7 @@
       <c r="C42" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F42" s="12"/>
+      <c r="F42" s="14"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
@@ -1631,7 +1654,7 @@
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
-      <c r="F43" s="13"/>
+      <c r="F43" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>